<commit_message>
add mode-transistion documentation of transition excluded by design for completeness
</commit_message>
<xml_diff>
--- a/docs/design/pss/limit-logic/mode-transition/truth-table-mode-set-reset.xlsx
+++ b/docs/design/pss/limit-logic/mode-transition/truth-table-mode-set-reset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\240613_HFU_SMA_Master_Thesis\obat\docs\design\pss\control-logic\limit-logic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\240613_HFU_SMA_Master_Thesis\obat\docs\design\pss\limit-logic\mode-transition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A18A924-7554-4F34-A0C7-61062448FB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EE1886-17FD-462D-B0AB-44CD3122CF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC98877B-7BEB-4BB2-B5C5-766C6DD71E55}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="20">
   <si>
     <t>LCLE</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>UI</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -316,12 +319,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -356,12 +394,50 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -376,13 +452,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF3F3F3F"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color rgb="FF3F3F3F"/>
@@ -499,27 +568,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -577,8 +625,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N15" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" headerRowCellStyle="Output" dataCellStyle="Output">
-  <autoFilter ref="A1:N15" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N16" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" headerRowCellStyle="Output" dataCellStyle="Output">
+  <autoFilter ref="A1:N16" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{1D4D7CFA-EEFF-49CC-B6E3-CD37603DD213}" name="REF" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{E872F240-7070-487A-A7D1-E1B89183F30B}" name="LVLE" dataDxfId="15"/>
@@ -587,13 +635,13 @@
     <tableColumn id="5" xr3:uid="{F1D526A6-C7EC-4884-86E9-64A0A4604C76}" name="UCLE" dataDxfId="12"/>
     <tableColumn id="6" xr3:uid="{D0B5C53A-88DE-4A9E-976F-E36A9D1BA20B}" name="MSTT" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{E8A2B42D-CA06-4DC8-83BA-A70DFD2D6854}" name="MGTT" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{B2368061-9F18-4098-9A4F-4B06E760DF3C}" name="VC" dataDxfId="6" dataCellStyle="Output"/>
-    <tableColumn id="9" xr3:uid="{D8248A7F-5964-4738-95C1-27D91A1C0045}" name="LCLC" dataDxfId="5" dataCellStyle="Output"/>
-    <tableColumn id="10" xr3:uid="{0434A4F2-0D31-487B-8538-80040501D86F}" name="UCLC" dataDxfId="4" dataCellStyle="Output"/>
-    <tableColumn id="11" xr3:uid="{5AC7D3EE-81C7-4EBC-9BD0-7AE42A9E9FDC}" name="CC" dataDxfId="3" dataCellStyle="Output"/>
-    <tableColumn id="12" xr3:uid="{CF1A8950-CF2C-496F-A1FD-F8F7FAF8BC53}" name="LVLC" dataDxfId="2" dataCellStyle="Output"/>
-    <tableColumn id="13" xr3:uid="{AC990C43-4F8C-41A5-A109-40604E315B53}" name="UVLC" dataDxfId="0" dataCellStyle="Output"/>
-    <tableColumn id="14" xr3:uid="{8E911C9F-856A-4EA8-8118-CAA6EB0E94CF}" name="Excl. By Design" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{B2368061-9F18-4098-9A4F-4B06E760DF3C}" name="VC" dataDxfId="9" dataCellStyle="Output"/>
+    <tableColumn id="9" xr3:uid="{D8248A7F-5964-4738-95C1-27D91A1C0045}" name="LCLC" dataDxfId="8" dataCellStyle="Output"/>
+    <tableColumn id="10" xr3:uid="{0434A4F2-0D31-487B-8538-80040501D86F}" name="UCLC" dataDxfId="7" dataCellStyle="Output"/>
+    <tableColumn id="11" xr3:uid="{5AC7D3EE-81C7-4EBC-9BD0-7AE42A9E9FDC}" name="CC" dataDxfId="6" dataCellStyle="Output"/>
+    <tableColumn id="12" xr3:uid="{CF1A8950-CF2C-496F-A1FD-F8F7FAF8BC53}" name="LVLC" dataDxfId="5" dataCellStyle="Output"/>
+    <tableColumn id="13" xr3:uid="{AC990C43-4F8C-41A5-A109-40604E315B53}" name="UVLC" dataDxfId="4" dataCellStyle="Output"/>
+    <tableColumn id="14" xr3:uid="{8E911C9F-856A-4EA8-8118-CAA6EB0E94CF}" name="Excl. By Design" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -916,11 +964,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9A2F88-A748-47D6-928C-CABCC02F70E6}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,15 +1591,59 @@
         <v>5</v>
       </c>
     </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix limit-logic missing state transitions between limiting modi
The state transition, which transitions from the upper limit control directly to the lower limit control
and vice versa is introduced in this commit. The simulation revealed that the transition was indeed missing.
The transition ensures robustness that the correct mode will be active, when e.g. the current rapidly changes
and the transition to the 'normal' operating mode is skipped/missed.
</commit_message>
<xml_diff>
--- a/docs/design/pss/limit-logic/mode-transition/truth-table-mode-set-reset.xlsx
+++ b/docs/design/pss/limit-logic/mode-transition/truth-table-mode-set-reset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\240613_HFU_SMA_Master_Thesis\obat\docs\design\pss\limit-logic\mode-transition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EE1886-17FD-462D-B0AB-44CD3122CF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5D3D9D-58E5-4A32-822E-94A873D5B8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC98877B-7BEB-4BB2-B5C5-766C6DD71E55}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{CC98877B-7BEB-4BB2-B5C5-766C6DD71E55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="22">
   <si>
     <t>LCLE</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>UI</t>
+  </si>
+  <si>
+    <t>S/R</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -395,14 +401,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -625,8 +631,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N16" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" headerRowCellStyle="Output" dataCellStyle="Output">
-  <autoFilter ref="A1:N16" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" headerRowCellStyle="Output" dataCellStyle="Output">
+  <autoFilter ref="A1:N17" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{1D4D7CFA-EEFF-49CC-B6E3-CD37603DD213}" name="REF" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{E872F240-7070-487A-A7D1-E1B89183F30B}" name="LVLE" dataDxfId="15"/>
@@ -964,11 +970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9A2F88-A748-47D6-928C-CABCC02F70E6}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1219,9 @@
       <c r="H6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="J6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1255,7 +1263,9 @@
       <c r="I7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="K7" s="8" t="s">
         <v>18</v>
       </c>
@@ -1292,10 +1302,10 @@
         <v>18</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>18</v>
@@ -1503,7 +1513,9 @@
       <c r="K13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="M13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1545,7 +1557,9 @@
       <c r="L14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="8"/>
+      <c r="M14" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1582,56 +1596,100 @@
         <v>18</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M16" s="15" t="s">
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="14" t="s">
         <v>18</v>
       </c>
       <c r="N16" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="12" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>